<commit_message>
Fresh version for Clement
</commit_message>
<xml_diff>
--- a/confirmed_global.xlsx
+++ b/confirmed_global.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbenn\Documents\Personal\COVID competition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbenn\Documents\Personal\COVID competition\covid_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C47F4D7C-CE15-4414-8059-2E4C4E1E6266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B88EDB5-3E60-44C2-9603-37C40C628503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{397F144D-8BB4-4458-9007-5DC2E83C3F53}"/>
   </bookViews>
@@ -1193,18 +1193,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54361BFA-C994-4B10-8BA9-6C41EEFE09E2}">
-  <dimension ref="A1:CR265"/>
+  <dimension ref="A1:DA265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="CG1" workbookViewId="0">
+      <selection activeCell="CY7" sqref="CY7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="96" max="104" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1493,8 +1494,35 @@
       <c r="CR1" s="1">
         <v>43943</v>
       </c>
+      <c r="CS1" s="1">
+        <v>43944</v>
+      </c>
+      <c r="CT1" s="1">
+        <v>43945</v>
+      </c>
+      <c r="CU1" s="1">
+        <v>43946</v>
+      </c>
+      <c r="CV1" s="1">
+        <v>43947</v>
+      </c>
+      <c r="CW1" s="1">
+        <v>43948</v>
+      </c>
+      <c r="CX1" s="1">
+        <v>43949</v>
+      </c>
+      <c r="CY1" s="1">
+        <v>43950</v>
+      </c>
+      <c r="CZ1" s="1">
+        <v>43951</v>
+      </c>
+      <c r="DA1" s="1">
+        <v>43952</v>
+      </c>
     </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:105" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -1781,7 +1809,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:105" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -2068,7 +2096,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:105" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -2355,7 +2383,7 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:105" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -2642,7 +2670,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="6" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:105" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -2929,7 +2957,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:105" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -3216,7 +3244,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:105" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -3503,7 +3531,7 @@
         <v>3144</v>
       </c>
     </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:105" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -3790,7 +3818,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4080,7 +4108,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -4370,7 +4398,7 @@
         <v>2926</v>
       </c>
     </row>
-    <row r="12" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -4660,7 +4688,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -4950,7 +4978,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="14" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -5240,7 +5268,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="15" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -5530,7 +5558,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>

</xml_diff>